<commit_message>
salesforce URL updated 88to85, accepting the release popup which is displaying newly
</commit_message>
<xml_diff>
--- a/input/testdata/KONEMobileSiteSurvey_TestData.xlsx
+++ b/input/testdata/KONEMobileSiteSurvey_TestData.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\con_svijay02\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6924"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="1548" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Data" sheetId="5" r:id="rId1"/>
@@ -20,7 +15,8 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Mobile_Data!$A$1:$D$64</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:G3"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -413,28 +409,28 @@
     <t>b.mamtha@kone.com</t>
   </si>
   <si>
+    <t>con_bmamtha</t>
+  </si>
+  <si>
+    <t>Welcome@123</t>
+  </si>
+  <si>
+    <t>ATEST_CustomerContact_2106</t>
+  </si>
+  <si>
+    <t>ATEST_Street_2106</t>
+  </si>
+  <si>
+    <t>21062018</t>
+  </si>
+  <si>
+    <t>ATEST_City_2106</t>
+  </si>
+  <si>
     <t>Data@123</t>
   </si>
   <si>
-    <t>con_bmamtha</t>
-  </si>
-  <si>
-    <t>Welcome@123</t>
-  </si>
-  <si>
-    <t>Atest_06062018_1</t>
-  </si>
-  <si>
-    <t>ATEST_CustomerContact_2106</t>
-  </si>
-  <si>
-    <t>ATEST_Street_2106</t>
-  </si>
-  <si>
-    <t>21062018</t>
-  </si>
-  <si>
-    <t>ATEST_City_2106</t>
+    <t>Atest_28062018</t>
   </si>
 </sst>
 </file>
@@ -523,7 +519,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -536,6 +532,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -853,7 +850,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -881,14 +880,14 @@
       <c r="A2" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="11" t="s">
         <v>128</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -901,7 +900,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -938,22 +939,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>120</v>

</xml_diff>

<commit_message>
password for salesforce updated
</commit_message>
<xml_diff>
--- a/input/testdata/KONEMobileSiteSurvey_TestData.xlsx
+++ b/input/testdata/KONEMobileSiteSurvey_TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="1548" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="2316"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Data" sheetId="5" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Mobile_Data!$A$1:$D$64</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:G3"/>
+  <oleSize ref="A1:K6"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -427,10 +427,10 @@
     <t>ATEST_City_2106</t>
   </si>
   <si>
-    <t>Data@123</t>
-  </si>
-  <si>
     <t>Atest_28062018</t>
+  </si>
+  <si>
+    <t>Welcome@234</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -532,7 +532,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -850,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -880,8 +879,8 @@
       <c r="A2" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>133</v>
+      <c r="B2" s="11" t="s">
+        <v>134</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>127</v>
@@ -900,7 +899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -939,7 +938,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
included VbmobileSurveytoLinkOpportunity testcase in VBMobile and SalesforceSurveytoLinkOpportunity testcase for web
</commit_message>
<xml_diff>
--- a/input/testdata/KONEMobileSiteSurvey_TestData.xlsx
+++ b/input/testdata/KONEMobileSiteSurvey_TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="2316"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13308" windowHeight="1884" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Data" sheetId="5" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Mobile_Data!$A$1:$D$64</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K6"/>
+  <oleSize ref="A1:F7"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="141">
   <si>
     <t>Run_Browser</t>
   </si>
@@ -388,12 +388,6 @@
     <t>MSS_SelectPlannedTypes</t>
   </si>
   <si>
-    <t>Budget</t>
-  </si>
-  <si>
-    <t>Full</t>
-  </si>
-  <si>
     <t>SF_UserName</t>
   </si>
   <si>
@@ -415,22 +409,46 @@
     <t>Welcome@123</t>
   </si>
   <si>
-    <t>ATEST_CustomerContact_2106</t>
-  </si>
-  <si>
-    <t>ATEST_Street_2106</t>
-  </si>
-  <si>
     <t>21062018</t>
   </si>
   <si>
-    <t>ATEST_City_2106</t>
-  </si>
-  <si>
-    <t>Atest_28062018</t>
-  </si>
-  <si>
     <t>Welcome@234</t>
+  </si>
+  <si>
+    <t>LIS</t>
+  </si>
+  <si>
+    <t>LIO</t>
+  </si>
+  <si>
+    <t>MSS_SurveyType</t>
+  </si>
+  <si>
+    <t>ATEST_CustomerContact_LIO</t>
+  </si>
+  <si>
+    <t>ATEST_Street_LIO</t>
+  </si>
+  <si>
+    <t>ATEST_City_LIO</t>
+  </si>
+  <si>
+    <t>SF_Environment</t>
+  </si>
+  <si>
+    <t>FULL</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>ATEST_OPP_12072018_1</t>
+  </si>
+  <si>
+    <t>FRB Budget</t>
+  </si>
+  <si>
+    <t>FRB Full</t>
   </si>
 </sst>
 </file>
@@ -847,11 +865,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -859,104 +875,41 @@
     <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>128</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>120</v>
+      <c r="E2" s="4" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -967,9 +920,105 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
+            <xm:f>'-data-'!$H$2:$H$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
             <xm:f>'-data-'!$F$2:$F$3</xm:f>
           </x14:formula1>
-          <xm:sqref>G2</xm:sqref>
+          <xm:sqref>H2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'-data-'!$G$2:$G$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1818,10 +1867,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1832,9 +1881,11 @@
     <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1853,8 +1904,14 @@
       <c r="F1" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1871,10 +1928,16 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+      <c r="G2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1891,10 +1954,16 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+      <c r="G3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="C4" t="s">
         <v>101</v>
@@ -1903,7 +1972,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -1914,7 +1983,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -1925,7 +1994,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1936,7 +2005,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1944,7 +2013,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1952,17 +2021,17 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
created object to get taskid from mobile to web
</commit_message>
<xml_diff>
--- a/input/testdata/KONEMobileSiteSurvey_TestData.xlsx
+++ b/input/testdata/KONEMobileSiteSurvey_TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13308" windowHeight="1884" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13488" windowHeight="2700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Data" sheetId="5" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Mobile_Data!$A$1:$D$64</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:F7"/>
+  <oleSize ref="A1:G7"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -442,13 +442,13 @@
     <t>QA</t>
   </si>
   <si>
+    <t>FRB Budget</t>
+  </si>
+  <si>
+    <t>FRB Full</t>
+  </si>
+  <si>
     <t>ATEST_OPP_12072018_1</t>
-  </si>
-  <si>
-    <t>FRB Budget</t>
-  </si>
-  <si>
-    <t>FRB Full</t>
   </si>
 </sst>
 </file>
@@ -867,7 +867,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -934,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -978,7 +980,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
@@ -999,7 +1001,7 @@
         <v>134</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1928,7 +1930,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G2" t="s">
         <v>129</v>
@@ -1954,7 +1956,7 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G3" t="s">
         <v>130</v>

</xml_diff>

<commit_message>
included new method for linksurvey in sitesurveyhomepage and implemented @aftertest in web and implementing @aftertest in mobile
</commit_message>
<xml_diff>
--- a/input/testdata/KONEMobileSiteSurvey_TestData.xlsx
+++ b/input/testdata/KONEMobileSiteSurvey_TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13488" windowHeight="2700" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13488" windowHeight="2328" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Data" sheetId="5" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Mobile_Data!$A$1:$D$64</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:G7"/>
+  <oleSize ref="A1:G6"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -448,7 +448,7 @@
     <t>FRB Full</t>
   </si>
   <si>
-    <t>ATEST_OPP_12072018_1</t>
+    <t>Atest_28062018</t>
   </si>
 </sst>
 </file>
@@ -911,7 +911,7 @@
         <v>126</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing @aftertest in web
</commit_message>
<xml_diff>
--- a/input/testdata/KONEMobileSiteSurvey_TestData.xlsx
+++ b/input/testdata/KONEMobileSiteSurvey_TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13488" windowHeight="2328" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10248" windowHeight="3708" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Data" sheetId="5" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Mobile_Data!$A$1:$D$64</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:G6"/>
+  <oleSize ref="A1:C9"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -202,12 +202,6 @@
     <t>Machine room safety balustrades</t>
   </si>
   <si>
-    <t>Machine room door width</t>
-  </si>
-  <si>
-    <t>Machine room door height</t>
-  </si>
-  <si>
     <t>Trapdoor</t>
   </si>
   <si>
@@ -367,9 +361,6 @@
     <t>Branch Number</t>
   </si>
   <si>
-    <t>Frontline Data OMA</t>
-  </si>
-  <si>
     <t>Required Field</t>
   </si>
   <si>
@@ -449,6 +440,15 @@
   </si>
   <si>
     <t>Atest_28062018</t>
+  </si>
+  <si>
+    <t>Frontline Data</t>
+  </si>
+  <si>
+    <t>Machine Room door or hatch height</t>
+  </si>
+  <si>
+    <t>Machine Room door or hatch width</t>
   </si>
 </sst>
 </file>
@@ -882,36 +882,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -936,7 +936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -960,7 +960,7 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -975,33 +975,33 @@
         <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1032,9 +1032,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1047,41 +1047,41 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
         <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D3">
         <v>13</v>
@@ -1089,13 +1089,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
         <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D4" t="s">
         <v>1</v>
@@ -1103,13 +1103,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
         <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
@@ -1117,13 +1117,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
         <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D6" t="s">
         <v>1</v>
@@ -1131,13 +1131,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
         <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D7" t="s">
         <v>2</v>
@@ -1145,27 +1145,27 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
         <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
         <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D9" t="s">
         <v>1</v>
@@ -1173,27 +1173,27 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B11" t="s">
         <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D11">
         <v>15</v>
@@ -1201,13 +1201,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
         <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D12">
         <v>1500</v>
@@ -1215,13 +1215,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B13" t="s">
         <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -1229,13 +1229,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B14" t="s">
         <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D14">
         <v>1500</v>
@@ -1243,13 +1243,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B15" t="s">
         <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D15">
         <v>2000</v>
@@ -1257,13 +1257,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
         <v>90</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" t="s">
-        <v>92</v>
       </c>
       <c r="D16">
         <v>1500</v>
@@ -1271,13 +1271,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B17" t="s">
         <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D17">
         <v>1800</v>
@@ -1285,27 +1285,27 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B18" t="s">
         <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B19" t="s">
         <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D19">
         <v>300</v>
@@ -1313,13 +1313,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
         <v>84</v>
-      </c>
-      <c r="B20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" t="s">
-        <v>86</v>
       </c>
       <c r="D20">
         <v>310</v>
@@ -1327,13 +1327,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B21" t="s">
         <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D21">
         <v>320</v>
@@ -1341,13 +1341,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B22" t="s">
         <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D22">
         <v>330</v>
@@ -1355,69 +1355,69 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B23" t="s">
         <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s">
         <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B25" t="s">
         <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B26" t="s">
         <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
         <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D27" t="s">
         <v>2</v>
@@ -1425,30 +1425,30 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B28" t="s">
         <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B29" t="s">
         <v>53</v>
       </c>
       <c r="C29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1456,10 +1456,10 @@
         <v>47</v>
       </c>
       <c r="B30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D30">
         <v>2009</v>
@@ -1473,10 +1473,10 @@
         <v>40</v>
       </c>
       <c r="C31" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1487,10 +1487,10 @@
         <v>40</v>
       </c>
       <c r="C32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1501,10 +1501,10 @@
         <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1515,7 +1515,7 @@
         <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>59</v>
+        <v>139</v>
       </c>
       <c r="D34">
         <v>2000</v>
@@ -1529,7 +1529,7 @@
         <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>58</v>
+        <v>140</v>
       </c>
       <c r="D35">
         <v>1200</v>
@@ -1872,7 +1872,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1895,22 +1895,22 @@
         <v>8</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1921,7 +1921,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="D2" t="s">
         <v>40</v>
@@ -1930,13 +1930,13 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1947,7 +1947,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
         <v>36</v>
@@ -1956,19 +1956,19 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D4" t="s">
         <v>53</v>
@@ -1979,10 +1979,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1990,10 +1990,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -2001,7 +2001,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
@@ -2012,7 +2012,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
including training app and fixing the resetapp
</commit_message>
<xml_diff>
--- a/input/testdata/KONEMobileSiteSurvey_TestData.xlsx
+++ b/input/testdata/KONEMobileSiteSurvey_TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10092" windowHeight="1932"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10116" windowHeight="3132" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Data" sheetId="5" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Mobile_Data!$A$1:$D$64</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:F4"/>
+  <oleSize ref="A1:E9"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -445,7 +445,7 @@
     <t>ATEST_City</t>
   </si>
   <si>
-    <t>Atest_28062018</t>
+    <t>ATEST_OPP_12072018_1</t>
   </si>
 </sst>
 </file>
@@ -864,7 +864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -908,7 +908,7 @@
         <v>123</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -933,7 +933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>